<commit_message>
removed word cache file
</commit_message>
<xml_diff>
--- a/FinalProposal/NeedMatrix.xlsx
+++ b/FinalProposal/NeedMatrix.xlsx
@@ -274,8 +274,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -295,13 +311,29 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -876,7 +908,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E2" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>